<commit_message>
Separate two different PCB - just 2 KiCad projects - buttons on left side or buttons next to joystick
</commit_message>
<xml_diff>
--- a/hw/display_bom.xlsx
+++ b/hw/display_bom.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michal\Desktop\semestralni prace\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michal\Desktop\semestralni prace\sw\display_repository\hw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
     <sheet name="List2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -191,7 +191,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -236,7 +236,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8"/>
@@ -521,7 +521,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Edit values of capacitors near tone generator + updated BOM + rename casing folder
</commit_message>
<xml_diff>
--- a/hw/display_bom.xlsx
+++ b/hw/display_bom.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="52">
   <si>
     <t>2,2uF/10V</t>
   </si>
@@ -167,6 +167,21 @@
   </si>
   <si>
     <t>Hasl, FR-4, 47x152mm</t>
+  </si>
+  <si>
+    <t>1800pF</t>
+  </si>
+  <si>
+    <t>2200pF</t>
+  </si>
+  <si>
+    <t>2700pF</t>
+  </si>
+  <si>
+    <t>3300pF</t>
+  </si>
+  <si>
+    <t>3900pF</t>
   </si>
 </sst>
 </file>
@@ -175,7 +190,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
-    <numFmt numFmtId="173" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -333,7 +348,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -352,7 +367,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -633,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,6 +1226,97 @@
       <c r="D32" s="14">
         <f>SUM(D2:D31)</f>
         <v>22.023044890999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40">
+        <v>2524826</v>
+      </c>
+      <c r="D40">
+        <v>0.248</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41">
+        <v>2496845</v>
+      </c>
+      <c r="D41">
+        <v>0.185</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42">
+        <v>2524833</v>
+      </c>
+      <c r="D42">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43">
+        <v>2496853</v>
+      </c>
+      <c r="D43">
+        <v>0.182</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44">
+        <v>2524841</v>
+      </c>
+      <c r="D44">
+        <v>0.248</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <f>SUM(D40:D44)</f>
+        <v>1.139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>